<commit_message>
Add emotional responses when Rando is not in the right mood
</commit_message>
<xml_diff>
--- a/Rando-Database.xlsx
+++ b/Rando-Database.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -399,17 +399,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>puppies</t>
+          <t>cake</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>attracted</t>
+          <t>bae</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>liptard</t>
+          <t>suck</t>
         </is>
       </c>
     </row>
@@ -419,22 +419,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>upset</t>
+          <t>dismay</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>cats</t>
+          <t>like</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>kiss</t>
+          <t>attractive</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>schmuck</t>
+          <t>bitch</t>
         </is>
       </c>
     </row>
@@ -444,22 +444,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>devastate</t>
+          <t>heartbreaking</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>like</t>
+          <t>puppies</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>honey</t>
+          <t>attracted</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>fat</t>
+          <t>ass</t>
         </is>
       </c>
     </row>
@@ -469,22 +469,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>cheating</t>
+          <t>pathetic</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>passed</t>
+          <t>pizza</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>bae</t>
+          <t>cute</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>stupid</t>
+          <t>fatty</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>disturb</t>
+          <t>wound</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -504,12 +504,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>;)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>lazy</t>
+          <t>fuck</t>
         </is>
       </c>
     </row>
@@ -519,22 +519,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>heartbreaking</t>
+          <t>cheating</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>sunflower</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>sexy</t>
+          <t>cutie</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ass</t>
+          <t>faggot</t>
         </is>
       </c>
     </row>
@@ -544,22 +544,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>death</t>
+          <t>miserable</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>cats</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>babe</t>
+          <t>sexy</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>cunt</t>
+          <t>jerk</t>
         </is>
       </c>
     </row>
@@ -569,22 +569,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>dismay</t>
+          <t>stab</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>pizza</t>
+          <t>friends</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>attractive</t>
+          <t>babe</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>hate</t>
+          <t>dork</t>
         </is>
       </c>
     </row>
@@ -599,17 +599,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>friends</t>
+          <t>success</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>;)</t>
+          <t>crush</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>jerk</t>
+          <t>dumb</t>
         </is>
       </c>
     </row>
@@ -619,18 +619,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>hang over</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>cute</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>bitch</t>
+          <t>schmuck</t>
         </is>
       </c>
     </row>
@@ -640,18 +644,18 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>miserable</t>
+          <t>hang over</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>love</t>
+          <t>kiss</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>suck</t>
+          <t>hate</t>
         </is>
       </c>
     </row>
@@ -661,18 +665,18 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>sad</t>
+          <t>death</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>crush</t>
+          <t>baby</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>fatty</t>
+          <t>cunt</t>
         </is>
       </c>
     </row>
@@ -682,13 +686,13 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>stab</t>
+          <t>tragic</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>baby</t>
+          <t>love</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -703,18 +707,18 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>tragic</t>
+          <t>terrible</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>cutie</t>
+          <t>honey</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>faggot</t>
+          <t>liptard</t>
         </is>
       </c>
     </row>
@@ -724,14 +728,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>distress</t>
+          <t>worry</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>loser</t>
+          <t>stupid</t>
         </is>
       </c>
     </row>
@@ -741,14 +745,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>pathetic</t>
+          <t>devastate</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>dumb</t>
+          <t>loser</t>
         </is>
       </c>
     </row>
@@ -758,14 +762,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>wound</t>
+          <t>distress</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>dork</t>
+          <t>fat</t>
         </is>
       </c>
     </row>
@@ -775,14 +779,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>worry</t>
+          <t>disturb</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>fuck</t>
+          <t>lazy</t>
         </is>
       </c>
     </row>
@@ -792,7 +796,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>depress</t>
+          <t>upset</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -805,7 +809,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>terrible</t>
+          <t>depress</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>

</xml_diff>